<commit_message>
PCA y ANOVA avanzados
Identificacion de outliers y analisis exploratorio. Ajuste de modelos, comprobacion de asunciones
</commit_message>
<xml_diff>
--- a/datos/Datos TFM Alberto.xlsx
+++ b/datos/Datos TFM Alberto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\collf\Documents\GitHub\TFM-Ortiguilla\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BDD4DDC-E149-4F91-9A29-7D0E6AAA347F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB9EB66B-AEDC-4327-919A-11F78A61C2EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1CB412F8-9ABE-48C7-98C9-C1273AA5EDC5}"/>
   </bookViews>
@@ -842,7 +842,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -985,10 +985,10 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1039,12 +1039,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8523,7 +8524,7 @@
   <dimension ref="A1:W22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="W21" sqref="A1:W21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8534,8 +8535,7 @@
     <col min="6" max="13" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="14" max="17" width="11.26953125" customWidth="1"/>
     <col min="18" max="20" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.81640625" customWidth="1"/>
+    <col min="21" max="22" width="11.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.35">
@@ -8658,10 +8658,10 @@
         <v>8.6940000000000008</v>
       </c>
       <c r="V2">
+        <v>478.19999999999993</v>
+      </c>
+      <c r="W2">
         <v>260.2</v>
-      </c>
-      <c r="W2">
-        <v>478.19999999999993</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.35">
@@ -8713,10 +8713,10 @@
         <v>8.4495000000000005</v>
       </c>
       <c r="V3">
+        <v>459.2</v>
+      </c>
+      <c r="W3">
         <v>323.2</v>
-      </c>
-      <c r="W3">
-        <v>459.2</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.35">
@@ -8768,10 +8768,10 @@
         <v>7.6635</v>
       </c>
       <c r="V4">
+        <v>449.2</v>
+      </c>
+      <c r="W4">
         <v>463.2</v>
-      </c>
-      <c r="W4">
-        <v>449.2</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.35">
@@ -8823,10 +8823,10 @@
         <v>7.8285</v>
       </c>
       <c r="V5">
+        <v>403.2</v>
+      </c>
+      <c r="W5">
         <v>508.2</v>
-      </c>
-      <c r="W5">
-        <v>403.2</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.35">
@@ -8878,10 +8878,10 @@
         <v>7.74</v>
       </c>
       <c r="V6">
+        <v>403.2</v>
+      </c>
+      <c r="W6">
         <v>263.2</v>
-      </c>
-      <c r="W6">
-        <v>403.2</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.35">
@@ -8933,10 +8933,10 @@
         <v>8.5934999999999988</v>
       </c>
       <c r="V7">
+        <v>390.2</v>
+      </c>
+      <c r="W7">
         <v>483.19999999999993</v>
-      </c>
-      <c r="W7">
-        <v>390.2</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.35">
@@ -8988,10 +8988,10 @@
         <v>7.474499999999999</v>
       </c>
       <c r="V8">
+        <v>438.20000000000005</v>
+      </c>
+      <c r="W8">
         <v>274.2</v>
-      </c>
-      <c r="W8">
-        <v>438.20000000000005</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.35">
@@ -9007,12 +9007,12 @@
       <c r="D9">
         <v>19</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="74">
         <v>208.93784786641928</v>
       </c>
       <c r="F9" s="33"/>
       <c r="G9" s="33"/>
-      <c r="H9">
+      <c r="H9" s="74">
         <v>116.65609443726856</v>
       </c>
       <c r="I9">
@@ -9022,7 +9022,7 @@
       <c r="K9" s="33"/>
       <c r="L9" s="33"/>
       <c r="M9" s="33"/>
-      <c r="N9">
+      <c r="N9" s="74">
         <v>715.14712976362773</v>
       </c>
       <c r="O9">
@@ -9043,10 +9043,10 @@
         <v>6.5880000000000001</v>
       </c>
       <c r="V9">
+        <v>476.2</v>
+      </c>
+      <c r="W9">
         <v>274.2</v>
-      </c>
-      <c r="W9">
-        <v>476.2</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.35">
@@ -9080,7 +9080,7 @@
       <c r="N10">
         <v>276.49983735303687</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="74">
         <v>213.27172189241159</v>
       </c>
       <c r="P10" s="33"/>
@@ -9098,10 +9098,10 @@
         <v>7.9169999999999989</v>
       </c>
       <c r="V10">
+        <v>383.19999999999993</v>
+      </c>
+      <c r="W10">
         <v>502.20000000000005</v>
-      </c>
-      <c r="W10">
-        <v>383.19999999999993</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.35">
@@ -9153,10 +9153,10 @@
         <v>6.5939999999999994</v>
       </c>
       <c r="V11">
+        <v>453.2</v>
+      </c>
+      <c r="W11">
         <v>504.20000000000005</v>
-      </c>
-      <c r="W11">
-        <v>453.2</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.35">
@@ -9208,10 +9208,10 @@
         <v>8.6609999999999996</v>
       </c>
       <c r="V12">
+        <v>338.20000000000005</v>
+      </c>
+      <c r="W12">
         <v>215.19999999999993</v>
-      </c>
-      <c r="W12">
-        <v>338.20000000000005</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.35">
@@ -9263,10 +9263,10 @@
         <v>7.5735000000000001</v>
       </c>
       <c r="V13">
+        <v>301.19999999999993</v>
+      </c>
+      <c r="W13">
         <v>269.2</v>
-      </c>
-      <c r="W13">
-        <v>301.19999999999993</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.35">
@@ -9318,10 +9318,10 @@
         <v>7.8959999999999999</v>
       </c>
       <c r="V14">
+        <v>365.2</v>
+      </c>
+      <c r="W14">
         <v>499.2</v>
-      </c>
-      <c r="W14">
-        <v>365.2</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.35">
@@ -9373,10 +9373,10 @@
         <v>8.5724999999999998</v>
       </c>
       <c r="V15">
+        <v>372.2</v>
+      </c>
+      <c r="W15">
         <v>473.19999999999993</v>
-      </c>
-      <c r="W15">
-        <v>372.2</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.35">
@@ -9428,10 +9428,10 @@
         <v>8.1180000000000003</v>
       </c>
       <c r="V16">
+        <v>340.2</v>
+      </c>
+      <c r="W16">
         <v>378.19999999999993</v>
-      </c>
-      <c r="W16">
-        <v>340.2</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.35">
@@ -9452,7 +9452,7 @@
       </c>
       <c r="F17" s="33"/>
       <c r="G17" s="33"/>
-      <c r="H17">
+      <c r="H17" s="74">
         <v>110.46637472716887</v>
       </c>
       <c r="I17">
@@ -9483,10 +9483,10 @@
         <v>6.9990000000000006</v>
       </c>
       <c r="V17">
+        <v>420.20000000000005</v>
+      </c>
+      <c r="W17">
         <v>490.19999999999993</v>
-      </c>
-      <c r="W17">
-        <v>420.20000000000005</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.35">
@@ -9528,7 +9528,7 @@
       <c r="R18">
         <v>43.341451766953199</v>
       </c>
-      <c r="S18">
+      <c r="S18" s="74">
         <v>75.934574976122263</v>
       </c>
       <c r="T18">
@@ -9538,10 +9538,10 @@
         <v>6.5324999999999998</v>
       </c>
       <c r="V18">
+        <v>397.2</v>
+      </c>
+      <c r="W18">
         <v>442.20000000000005</v>
-      </c>
-      <c r="W18">
-        <v>397.2</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.35">
@@ -9593,10 +9593,10 @@
         <v>8.0730000000000004</v>
       </c>
       <c r="V19">
+        <v>366.20000000000005</v>
+      </c>
+      <c r="W19">
         <v>417.20000000000005</v>
-      </c>
-      <c r="W19">
-        <v>366.20000000000005</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.35">
@@ -9648,10 +9648,10 @@
         <v>7.1744999999999992</v>
       </c>
       <c r="V20">
+        <v>365.19999999999993</v>
+      </c>
+      <c r="W20">
         <v>423.2</v>
-      </c>
-      <c r="W20">
-        <v>365.19999999999993</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.35">
@@ -9675,7 +9675,7 @@
       <c r="H21">
         <v>74.095671718176504</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="74">
         <v>50.052624244975469</v>
       </c>
       <c r="J21" s="33"/>
@@ -9703,10 +9703,10 @@
         <v>5.5470000000000006</v>
       </c>
       <c r="V21">
+        <v>409.2</v>
+      </c>
+      <c r="W21">
         <v>340.2</v>
-      </c>
-      <c r="W21">
-        <v>409.2</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.35">
@@ -13575,7 +13575,7 @@
   <dimension ref="A1:W81"/>
   <sheetViews>
     <sheetView topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2:R41"/>
+      <selection activeCell="R16" sqref="R16:R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17441,8 +17441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D180DB6-3E30-40EF-BF18-C12BE3EB45CB}">
   <dimension ref="A1:W50"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25:Q26"/>
+    <sheetView topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q41" sqref="Q41:Q42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17467,16 +17467,16 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B1" s="14"/>
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
       <c r="K1" s="51" t="s">
         <v>72</v>
       </c>
@@ -18465,13 +18465,13 @@
       </c>
       <c r="I25" s="53"/>
       <c r="J25" s="46"/>
-      <c r="K25" s="55">
+      <c r="K25" s="54">
         <v>3.1095000000000002</v>
       </c>
       <c r="L25" s="37">
         <v>-28.385000000000002</v>
       </c>
-      <c r="M25" s="55">
+      <c r="M25" s="54">
         <f t="shared" ref="M25" si="34">AVERAGE(L25:L26)</f>
         <v>-26.92</v>
       </c>
@@ -18509,11 +18509,11 @@
       <c r="H26" s="53"/>
       <c r="I26" s="53"/>
       <c r="J26" s="46"/>
-      <c r="K26" s="55"/>
+      <c r="K26" s="54"/>
       <c r="L26" s="37">
         <v>-25.454999999999998</v>
       </c>
-      <c r="M26" s="55"/>
+      <c r="M26" s="54"/>
       <c r="N26" s="56"/>
       <c r="O26" s="57"/>
       <c r="P26" s="57"/>
@@ -19517,13 +19517,13 @@
       <c r="A49" s="8">
         <v>20</v>
       </c>
-      <c r="B49" s="55">
+      <c r="B49" s="54">
         <v>5.5470000000000006</v>
       </c>
       <c r="C49" s="37">
         <v>-20.824000000000002</v>
       </c>
-      <c r="D49" s="55">
+      <c r="D49" s="54">
         <f t="shared" si="65"/>
         <v>-20.604500000000002</v>
       </c>
@@ -19578,11 +19578,11 @@
       <c r="A50" s="8">
         <v>20</v>
       </c>
-      <c r="B50" s="55"/>
+      <c r="B50" s="54"/>
       <c r="C50" s="37">
         <v>-20.385000000000002</v>
       </c>
-      <c r="D50" s="55"/>
+      <c r="D50" s="54"/>
       <c r="E50" s="56"/>
       <c r="F50" s="57"/>
       <c r="G50" s="57"/>
@@ -19696,6 +19696,10 @@
     <mergeCell ref="M39:M40"/>
     <mergeCell ref="N41:N42"/>
     <mergeCell ref="N43:N44"/>
+    <mergeCell ref="M29:M30"/>
+    <mergeCell ref="M31:M32"/>
+    <mergeCell ref="M33:M34"/>
+    <mergeCell ref="M35:M36"/>
     <mergeCell ref="N3:N4"/>
     <mergeCell ref="N5:N6"/>
     <mergeCell ref="N7:N8"/>
@@ -19705,10 +19709,6 @@
     <mergeCell ref="N15:N16"/>
     <mergeCell ref="N17:N18"/>
     <mergeCell ref="N19:N20"/>
-    <mergeCell ref="M29:M30"/>
-    <mergeCell ref="M31:M32"/>
-    <mergeCell ref="M33:M34"/>
-    <mergeCell ref="M35:M36"/>
     <mergeCell ref="K45:K46"/>
     <mergeCell ref="K47:K48"/>
     <mergeCell ref="K49:K50"/>
@@ -19886,8 +19886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4763BB1F-A466-48F0-ADE4-9FFEFA23D264}">
   <dimension ref="A1:W42"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19:H20"/>
+    <sheetView topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17:Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20693,7 +20693,7 @@
       </c>
       <c r="I17" s="63"/>
       <c r="J17" s="65"/>
-      <c r="K17" s="55">
+      <c r="K17" s="54">
         <v>3.1095000000000002</v>
       </c>
       <c r="L17" s="38">
@@ -20737,7 +20737,7 @@
       <c r="H18" s="66"/>
       <c r="I18" s="63"/>
       <c r="J18" s="65"/>
-      <c r="K18" s="55"/>
+      <c r="K18" s="54"/>
       <c r="L18" s="38">
         <v>7.5310000000000002E-2</v>
       </c>
@@ -20753,7 +20753,7 @@
       <c r="A19" s="8">
         <v>9</v>
       </c>
-      <c r="B19" s="55">
+      <c r="B19" s="54">
         <v>7.9169999999999989</v>
       </c>
       <c r="C19" s="39">
@@ -20814,7 +20814,7 @@
       <c r="A20" s="8">
         <v>9</v>
       </c>
-      <c r="B20" s="55"/>
+      <c r="B20" s="54"/>
       <c r="C20" s="39">
         <v>7.0709999999999995E-2</v>
       </c>
@@ -22120,8 +22120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB3AB737-2DEC-402C-8DC2-07BEE529A9DE}">
   <dimension ref="A2:P61"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65:XFD65"/>
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -22402,7 +22402,7 @@
     <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="8"/>
       <c r="B20" s="25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C20" s="25"/>
       <c r="D20" s="25"/>
@@ -22411,7 +22411,7 @@
       <c r="G20" s="25"/>
       <c r="H20" s="25"/>
       <c r="I20" s="26" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J20" s="26"/>
       <c r="K20" s="26"/>
@@ -24306,8 +24306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13D15522-C470-413D-B51F-D9EA713DB163}">
   <dimension ref="A1:Q104"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26:G35"/>
+    <sheetView topLeftCell="A31" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="K40" sqref="K40:K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -26670,8 +26670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6935F02E-8B65-4A8C-9022-EC9B9FAD68E1}">
   <dimension ref="A2:O64"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L46" sqref="L46"/>
+    <sheetView topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36:J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -26839,7 +26839,7 @@
         <f t="shared" si="0"/>
         <v>48.40353390639924</v>
       </c>
-      <c r="D6" s="73">
+      <c r="D6" s="72">
         <f>AVERAGE(C6:C6)</f>
         <v>48.40353390639924</v>
       </c>
@@ -26878,7 +26878,7 @@
         <f t="shared" si="0"/>
         <v>72.185768863419298</v>
       </c>
-      <c r="D7" s="73"/>
+      <c r="D7" s="72"/>
       <c r="E7" s="49"/>
       <c r="F7" s="44"/>
       <c r="G7" s="46"/>
@@ -26922,7 +26922,7 @@
         <f t="shared" si="1"/>
         <v>28.632760267430751</v>
       </c>
-      <c r="J8" s="72">
+      <c r="J8" s="73">
         <f t="shared" ref="J8" si="6">AVERAGE(I8:I9)</f>
         <v>31.593600764087867</v>
       </c>
@@ -26955,7 +26955,7 @@
         <f t="shared" si="1"/>
         <v>34.55444126074498</v>
       </c>
-      <c r="J9" s="72"/>
+      <c r="J9" s="73"/>
       <c r="K9" s="46"/>
       <c r="L9" s="44"/>
       <c r="M9" s="46"/>
@@ -26971,7 +26971,7 @@
         <f t="shared" si="0"/>
         <v>188.61365807067813</v>
       </c>
-      <c r="D10" s="73">
+      <c r="D10" s="72">
         <f>AVERAGE(C11:C11)</f>
         <v>59.912607449856743</v>
       </c>
@@ -26988,7 +26988,7 @@
         <f t="shared" si="1"/>
         <v>26.770296084049665</v>
       </c>
-      <c r="J10" s="72">
+      <c r="J10" s="73">
         <f t="shared" ref="J10" si="8">AVERAGE(I10:I11)</f>
         <v>32.691977077363894</v>
       </c>
@@ -27010,7 +27010,7 @@
         <f t="shared" si="0"/>
         <v>59.912607449856743</v>
       </c>
-      <c r="D11" s="73"/>
+      <c r="D11" s="72"/>
       <c r="E11" s="49"/>
       <c r="F11" s="44"/>
       <c r="G11" s="46"/>
@@ -27021,7 +27021,7 @@
         <f t="shared" si="1"/>
         <v>38.613658070678127</v>
       </c>
-      <c r="J11" s="72"/>
+      <c r="J11" s="73"/>
       <c r="K11" s="46"/>
       <c r="L11" s="44"/>
       <c r="M11" s="46"/>
@@ -27054,7 +27054,7 @@
         <f t="shared" si="1"/>
         <v>52.271728748806112</v>
       </c>
-      <c r="J12" s="72">
+      <c r="J12" s="73">
         <f t="shared" ref="J12" si="12">AVERAGE(I12:I13)</f>
         <v>50.934574976122249</v>
       </c>
@@ -27087,7 +27087,7 @@
         <f t="shared" si="1"/>
         <v>49.597421203438394</v>
       </c>
-      <c r="J13" s="72"/>
+      <c r="J13" s="73"/>
       <c r="K13" s="46"/>
       <c r="L13" s="44"/>
       <c r="M13" s="46"/>
@@ -27396,7 +27396,7 @@
         <f t="shared" si="1"/>
         <v>52.46275071633238</v>
       </c>
-      <c r="J22" s="72">
+      <c r="J22" s="73">
         <f t="shared" ref="J22:J32" si="32">AVERAGE(I22:I23)</f>
         <v>48.522922636103146</v>
       </c>
@@ -27429,7 +27429,7 @@
         <f t="shared" si="1"/>
         <v>44.58309455587392</v>
       </c>
-      <c r="J23" s="72"/>
+      <c r="J23" s="73"/>
       <c r="K23" s="46"/>
       <c r="L23" s="44"/>
       <c r="M23" s="46"/>
@@ -27882,7 +27882,7 @@
         <f t="shared" si="1"/>
         <v>76.053963705826177</v>
       </c>
-      <c r="J36" s="73">
+      <c r="J36" s="72">
         <f t="shared" si="22"/>
         <v>75.934574976122263</v>
       </c>
@@ -27915,7 +27915,7 @@
         <f t="shared" si="1"/>
         <v>75.815186246418349</v>
       </c>
-      <c r="J37" s="73"/>
+      <c r="J37" s="72"/>
       <c r="K37" s="46"/>
       <c r="L37" s="44"/>
       <c r="M37" s="46"/>
@@ -27948,7 +27948,7 @@
         <f t="shared" si="1"/>
         <v>47.734957020057301</v>
       </c>
-      <c r="J38" s="72">
+      <c r="J38" s="73">
         <f t="shared" si="26"/>
         <v>47.949856733524356</v>
       </c>
@@ -27981,7 +27981,7 @@
         <f t="shared" si="1"/>
         <v>48.164756446991412</v>
       </c>
-      <c r="J39" s="72"/>
+      <c r="J39" s="73"/>
       <c r="K39" s="46"/>
       <c r="L39" s="44"/>
       <c r="M39" s="46"/>
@@ -28080,7 +28080,7 @@
         <f t="shared" si="1"/>
         <v>53.131327602674311</v>
       </c>
-      <c r="J42" s="72">
+      <c r="J42" s="73">
         <f t="shared" si="28"/>
         <v>53.059694364851964</v>
       </c>
@@ -28113,7 +28113,7 @@
         <f t="shared" si="1"/>
         <v>52.988061127029617</v>
       </c>
-      <c r="J43" s="72"/>
+      <c r="J43" s="73"/>
       <c r="K43" s="46"/>
       <c r="L43" s="44"/>
       <c r="M43" s="46"/>
@@ -28256,6 +28256,9 @@
     <mergeCell ref="J10:J11"/>
     <mergeCell ref="K10:K11"/>
     <mergeCell ref="L4:L13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="K12:K13"/>
     <mergeCell ref="M4:M13"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:E7"/>
@@ -28272,14 +28275,6 @@
     <mergeCell ref="J4:J5"/>
     <mergeCell ref="K4:K5"/>
     <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F23"/>
-    <mergeCell ref="G14:G23"/>
-    <mergeCell ref="J14:J15"/>
     <mergeCell ref="K14:K15"/>
     <mergeCell ref="L14:L23"/>
     <mergeCell ref="M14:M23"/>
@@ -28291,6 +28286,11 @@
     <mergeCell ref="E18:E19"/>
     <mergeCell ref="J18:J19"/>
     <mergeCell ref="K18:K19"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F23"/>
+    <mergeCell ref="G14:G23"/>
+    <mergeCell ref="J14:J15"/>
     <mergeCell ref="D30:D31"/>
     <mergeCell ref="E30:E31"/>
     <mergeCell ref="J30:J31"/>
@@ -28329,6 +28329,8 @@
     <mergeCell ref="G34:G43"/>
     <mergeCell ref="J34:J35"/>
     <mergeCell ref="K34:K35"/>
+    <mergeCell ref="J42:J43"/>
+    <mergeCell ref="K42:K43"/>
     <mergeCell ref="L34:L43"/>
     <mergeCell ref="M34:M43"/>
     <mergeCell ref="D36:D37"/>
@@ -28345,8 +28347,6 @@
     <mergeCell ref="K40:K41"/>
     <mergeCell ref="D42:D43"/>
     <mergeCell ref="E42:E43"/>
-    <mergeCell ref="J42:J43"/>
-    <mergeCell ref="K42:K43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>